<commit_message>
Add the price in the email
</commit_message>
<xml_diff>
--- a/binance_ETHUSDT_MACD.xlsx
+++ b/binance_ETHUSDT_MACD.xlsx
@@ -472,17 +472,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>136.25000000</t>
+          <t>134.41000000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>136.42000000</t>
+          <t>137.54000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>40862.50242000</t>
+          <t>82844.02124000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -490,20 +490,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>5721842.07121670</t>
+          <t>11463838.27860240</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>11313</v>
+        <v>22364</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>18580.61358000</t>
+          <t>39241.33434000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>2604670.37233260</t>
+          <t>5432951.71095180</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>-17.7649346494116</v>
+        <v>-17.67558992006687</v>
       </c>
       <c r="Q2" t="n">
-        <v>-11.9389179756324</v>
+        <v>-11.92104902976346</v>
       </c>
       <c r="R2" t="n">
-        <v>-5.826016673779197</v>
+        <v>-5.754540890303412</v>
       </c>
     </row>
     <row r="3">

</xml_diff>